<commit_message>
Changed layout of charts and commented code
</commit_message>
<xml_diff>
--- a/ColliderTests.xlsx
+++ b/ColliderTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayla\Desktop\advanced-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF9BF77-3CBA-4F25-B494-4E3B30F409AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADCF1CD-90AE-4B0A-AFBF-F532BEF48E4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,19 +138,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -167,7 +161,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Different Collider Types</a:t>
+              <a:t>Different Collider Types Sorted by Objects</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -185,19 +179,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -221,41 +209,13 @@
             <c:v>AABB</c:v>
           </c:tx>
           <c:spPr>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="0"/>
-                    <a:lumOff val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="42000">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="0"/>
-                    <a:lumOff val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:path path="circle">
-                <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-              </a:path>
-              <a:tileRect/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -312,40 +272,13 @@
             <c:v>OBB</c:v>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="0"/>
-                    <a:lumOff val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="25000">
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="0"/>
-                    <a:lumOff val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:path path="circle">
-                <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-              </a:path>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -402,41 +335,13 @@
             <c:v>Mix</c:v>
           </c:tx>
           <c:spPr>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="0"/>
-                    <a:lumOff val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="27000">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="0"/>
-                    <a:lumOff val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:path path="circle">
-                <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-              </a:path>
-              <a:tileRect/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
@@ -474,8 +379,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="100"/>
-        <c:overlap val="-24"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
         <c:axId val="295166991"/>
         <c:axId val="299501887"/>
       </c:barChart>
@@ -492,11 +397,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="54000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -510,8 +415,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -541,9 +447,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -558,10 +464,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -589,10 +496,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -622,8 +530,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -648,16 +557,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.38744806081801075"/>
-          <c:y val="0.9147925834752455"/>
-          <c:w val="0.21602122622955508"/>
-          <c:h val="6.0225260921613927E-2"/>
-        </c:manualLayout>
-      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -673,8 +572,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -691,28 +591,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -755,19 +644,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -784,7 +667,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Different Collider Types</a:t>
+              <a:t>Different Collider Types Sorted by Colliders</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -802,19 +685,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -838,41 +715,13 @@
             <c:v>500 Objects</c:v>
           </c:tx>
           <c:spPr>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="0"/>
-                    <a:lumOff val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="42000">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="0"/>
-                    <a:lumOff val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:path path="circle">
-                <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-              </a:path>
-              <a:tileRect/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -923,40 +772,13 @@
             <c:v>1000 Objects</c:v>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="0"/>
-                    <a:lumOff val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="25000">
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="0"/>
-                    <a:lumOff val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:path path="circle">
-                <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-              </a:path>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -1007,41 +829,13 @@
             <c:v>1500 Objects</c:v>
           </c:tx>
           <c:spPr>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="0"/>
-                    <a:lumOff val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="27000">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="0"/>
-                    <a:lumOff val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:path path="circle">
-                <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-              </a:path>
-              <a:tileRect/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -1092,41 +886,13 @@
             <c:v>2000 Objects</c:v>
           </c:tx>
           <c:spPr>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="0"/>
-                    <a:lumOff val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="35000">
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="0"/>
-                    <a:lumOff val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:path path="circle">
-                <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-              </a:path>
-              <a:tileRect/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
@@ -1161,8 +927,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="100"/>
-        <c:overlap val="-24"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
         <c:axId val="295166991"/>
         <c:axId val="299501887"/>
       </c:barChart>
@@ -1179,11 +945,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="54000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1197,8 +963,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1228,9 +995,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1245,10 +1012,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1276,10 +1044,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1309,8 +1078,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1335,16 +1105,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.20806568116315158"/>
-          <c:y val="0.91122370410336828"/>
-          <c:w val="0.61783847182589913"/>
-          <c:h val="6.0225260921613927E-2"/>
-        </c:manualLayout>
-      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1360,8 +1120,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1378,28 +1139,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1502,33 +1252,35 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1536,34 +1288,26 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -1572,8 +1316,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1592,6 +1337,14 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1600,35 +1353,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1640,31 +1393,30 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1680,18 +1432,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1701,20 +1456,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1725,17 +1480,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1744,13 +1499,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1762,22 +1518,28 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1789,16 +1551,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -1807,17 +1570,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1826,16 +1589,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1844,26 +1608,27 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1871,21 +1636,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1893,14 +1648,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1912,19 +1667,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1933,13 +1681,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1948,8 +1697,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1959,7 +1709,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1967,9 +1717,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1980,8 +1730,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1991,40 +1742,48 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2032,34 +1791,26 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -2068,8 +1819,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2088,6 +1840,14 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -2096,35 +1856,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2136,31 +1896,30 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2176,18 +1935,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2197,20 +1959,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2221,17 +1983,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2240,13 +2002,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2258,22 +2021,28 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2285,16 +2054,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -2303,17 +2073,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -2322,16 +2092,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -2340,26 +2111,27 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -2367,21 +2139,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2389,14 +2151,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2408,19 +2170,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2429,13 +2184,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2444,8 +2200,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2455,7 +2212,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2463,9 +2220,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2476,8 +2233,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2487,8 +2245,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2499,14 +2263,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2533,16 +2297,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2837,8 +2601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>